<commit_message>
Refined implementation of SIGHUP reload signal based on Asset
</commit_message>
<xml_diff>
--- a/Data/Config_Dev.xlsx
+++ b/Data/Config_Dev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github.com\rpapub\ProlificQuasar\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FF2236-7D5F-4578-B41E-7DC38607E75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B5AAD9-EC2C-4859-94C5-850B46936A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1950" windowWidth="24210" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>ProlificQuasar_SIGHUP</t>
+  </si>
+  <si>
+    <t>AssetnameReloadSignal</t>
   </si>
   <si>
     <t>foo</t>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -592,16 +595,25 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26">
+      <c r="C3" s="4"/>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
-        <v>44</v>
+      <c r="B5" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1590,6 +1602,7 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2765,7 +2778,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>